<commit_message>
update code with removing tally matching heads and add todays date in date column and Jounral in Vch Name Column
</commit_message>
<xml_diff>
--- a/tally_icm_heads.xlsx
+++ b/tally_icm_heads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6fafba0055b58585/Python labs/tally entry JV format/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6fafba0055b58585/Automation/git_repo/icm_to_tdl_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="14_{625B3B86-C10E-421B-9B82-CC87EBC798B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AED3C85-227A-4759-AF2F-337EF7C6C0F6}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="14_{625B3B86-C10E-421B-9B82-CC87EBC798B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A916B66-4B60-4DFB-989C-67152CC91F1A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{3395FFBA-FE70-4DC8-A3D5-81A26907D2A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3395FFBA-FE70-4DC8-A3D5-81A26907D2A2}"/>
   </bookViews>
   <sheets>
     <sheet name="icm_tally_heads" sheetId="1" r:id="rId1"/>
@@ -1812,11 +1812,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30BA155A-597B-48F1-BBC3-5AB5AF1C4A8B}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:B500"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A434" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B509" sqref="B509"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5402,319 +5403,319 @@
         <v>444</v>
       </c>
     </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A448" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B448" s="3"/>
     </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A449" s="6" t="s">
         <v>153</v>
       </c>
       <c r="B449" s="3"/>
     </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A450" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B450" s="3"/>
     </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451" s="6" t="s">
         <v>154</v>
       </c>
       <c r="B451" s="3"/>
     </row>
-    <row r="452" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452" s="6" t="s">
         <v>155</v>
       </c>
       <c r="B452" s="3"/>
     </row>
-    <row r="453" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A453" s="6" t="s">
         <v>156</v>
       </c>
       <c r="B453" s="3"/>
     </row>
-    <row r="454" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A454" s="6" t="s">
         <v>161</v>
       </c>
       <c r="B454" s="3"/>
     </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A455" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B455" s="3"/>
     </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A456" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B456" s="4"/>
     </row>
-    <row r="457" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A457" s="6" t="s">
         <v>264</v>
       </c>
       <c r="B457" s="3"/>
     </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A458" s="6" t="s">
         <v>163</v>
       </c>
       <c r="B458" s="3"/>
     </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A459" s="6" t="s">
         <v>165</v>
       </c>
       <c r="B459" s="3"/>
     </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A460" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B460" s="3"/>
     </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A461" s="6" t="s">
         <v>169</v>
       </c>
       <c r="B461" s="3"/>
     </row>
-    <row r="462" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A462" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B462" s="3"/>
     </row>
-    <row r="463" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A463" s="6" t="s">
         <v>270</v>
       </c>
       <c r="B463" s="3"/>
     </row>
-    <row r="464" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A464" s="6" t="s">
         <v>271</v>
       </c>
       <c r="B464" s="3"/>
     </row>
-    <row r="465" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A465" s="6" t="s">
         <v>273</v>
       </c>
       <c r="B465" s="3"/>
     </row>
-    <row r="466" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A466" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B466" s="3"/>
     </row>
-    <row r="467" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A467" s="6" t="s">
         <v>224</v>
       </c>
       <c r="B467" s="3"/>
     </row>
-    <row r="468" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A468" s="6" t="s">
         <v>258</v>
       </c>
       <c r="B468" s="3"/>
     </row>
-    <row r="469" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A469" s="6" t="s">
         <v>234</v>
       </c>
       <c r="B469" s="3"/>
     </row>
-    <row r="470" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A470" s="6" t="s">
         <v>235</v>
       </c>
       <c r="B470" s="3"/>
     </row>
-    <row r="471" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A471" s="6" t="s">
         <v>235</v>
       </c>
       <c r="B471" s="3"/>
     </row>
-    <row r="472" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A472" s="6" t="s">
         <v>309</v>
       </c>
       <c r="B472" s="3"/>
     </row>
-    <row r="473" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A473" s="6" t="s">
         <v>237</v>
       </c>
       <c r="B473" s="3"/>
     </row>
-    <row r="474" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A474" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B474" s="3"/>
     </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A475" s="6" t="s">
         <v>278</v>
       </c>
       <c r="B475" s="4"/>
     </row>
-    <row r="476" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A476" s="6" t="s">
         <v>279</v>
       </c>
       <c r="B476" s="4"/>
     </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A477" s="6" t="s">
         <v>280</v>
       </c>
       <c r="B477" s="4"/>
     </row>
-    <row r="478" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A478" s="6" t="s">
         <v>310</v>
       </c>
       <c r="B478" s="4"/>
     </row>
-    <row r="479" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A479" s="6" t="s">
         <v>281</v>
       </c>
       <c r="B479" s="4"/>
     </row>
-    <row r="480" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A480" s="6" t="s">
         <v>281</v>
       </c>
       <c r="B480" s="4"/>
     </row>
-    <row r="481" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A481" s="6" t="s">
         <v>247</v>
       </c>
       <c r="B481" s="4"/>
     </row>
-    <row r="482" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A482" s="6" t="s">
         <v>282</v>
       </c>
       <c r="B482" s="4"/>
     </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A483" s="6" t="s">
         <v>283</v>
       </c>
       <c r="B483" s="4"/>
     </row>
-    <row r="484" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A484" s="6" t="s">
         <v>294</v>
       </c>
       <c r="B484" s="4"/>
     </row>
-    <row r="485" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A485" s="6" t="s">
         <v>312</v>
       </c>
       <c r="B485" s="4"/>
     </row>
-    <row r="486" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A486" s="6" t="s">
         <v>295</v>
       </c>
       <c r="B486" s="4"/>
     </row>
-    <row r="487" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A487" s="6" t="s">
         <v>296</v>
       </c>
       <c r="B487" s="4"/>
     </row>
-    <row r="488" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A488" s="6" t="s">
         <v>297</v>
       </c>
       <c r="B488" s="4"/>
     </row>
-    <row r="489" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A489" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B489" s="4"/>
     </row>
-    <row r="490" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A490" s="6" t="s">
         <v>221</v>
       </c>
       <c r="B490" s="4"/>
     </row>
-    <row r="491" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A491" s="6" t="s">
         <v>180</v>
       </c>
       <c r="B491" s="4"/>
     </row>
-    <row r="492" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A492" s="6" t="s">
         <v>182</v>
       </c>
       <c r="B492" s="4"/>
     </row>
-    <row r="493" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A493" s="6" t="s">
         <v>185</v>
       </c>
       <c r="B493" s="4"/>
     </row>
-    <row r="494" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A494" s="6" t="s">
         <v>167</v>
       </c>
       <c r="B494" s="4"/>
     </row>
-    <row r="495" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A495" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B495" s="4"/>
     </row>
-    <row r="496" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A496" s="6" t="s">
         <v>243</v>
       </c>
       <c r="B496" s="4"/>
     </row>
-    <row r="497" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A497" s="6" t="s">
         <v>200</v>
       </c>
       <c r="B497" s="4"/>
     </row>
-    <row r="498" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A498" s="6" t="s">
         <v>201</v>
       </c>
       <c r="B498" s="4"/>
     </row>
-    <row r="499" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A499" s="6" t="s">
         <v>119</v>
       </c>
       <c r="B499" s="4"/>
     </row>
-    <row r="500" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A500" s="6" t="s">
         <v>143</v>
       </c>
@@ -5722,6 +5723,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:B500" xr:uid="{30BA155A-597B-48F1-BBC3-5AB5AF1C4A8B}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B500">
       <sortCondition ref="B1:B499"/>
     </sortState>

</xml_diff>